<commit_message>
mass Operation for tax exempt
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateUS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateUS.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D0C14CDF-E306-4E1A-8278-68423A411611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="4635" tabRatio="363"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23280" windowHeight="13224" tabRatio="363" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass Change" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G13"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>Cmr No.</t>
   </si>
@@ -249,12 +250,18 @@
   </si>
   <si>
     <t>ENTERPRISE</t>
+  </si>
+  <si>
+    <t>Tax Exempt Status</t>
+  </si>
+  <si>
+    <t>TAX_EXEMPT_STATUS_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,6 +343,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -355,7 +430,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -643,15 +718,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AO502"/>
+  <dimension ref="A1:AP502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>40</v>
@@ -724,11 +801,12 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,1507 +928,1510 @@
         <v>70</v>
       </c>
       <c r="AO2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="6"/>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="6"/>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="6"/>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
     </row>
-    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
     </row>
-    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
     </row>
-    <row r="145" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
     </row>
-    <row r="146" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
     </row>
-    <row r="147" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
     </row>
-    <row r="148" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
     </row>
-    <row r="149" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
     </row>
-    <row r="150" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
     </row>
-    <row r="151" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
     </row>
-    <row r="152" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
     </row>
-    <row r="153" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
     </row>
-    <row r="154" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
     </row>
-    <row r="155" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
     </row>
-    <row r="156" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
     </row>
-    <row r="157" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
     </row>
-    <row r="158" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
     </row>
-    <row r="159" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
     </row>
-    <row r="160" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
     </row>
-    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
     </row>
-    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
     </row>
-    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
     </row>
-    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
     </row>
-    <row r="165" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
     </row>
-    <row r="166" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
     </row>
-    <row r="167" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
     </row>
-    <row r="168" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
     </row>
-    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
     </row>
-    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
     </row>
-    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
     </row>
-    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
     </row>
-    <row r="173" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
     </row>
-    <row r="174" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
     </row>
-    <row r="175" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
     </row>
-    <row r="176" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="6"/>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="6"/>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="6"/>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="6"/>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="6"/>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="6"/>
     </row>
-    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="6"/>
     </row>
-    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="6"/>
     </row>
-    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="6"/>
     </row>
-    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="6"/>
     </row>
-    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="6"/>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="6"/>
     </row>
-    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="6"/>
     </row>
-    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
     </row>
-    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="6"/>
     </row>
-    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="6"/>
     </row>
-    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="6"/>
     </row>
-    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="6"/>
     </row>
-    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="6"/>
     </row>
-    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
     </row>
-    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="6"/>
     </row>
-    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="6"/>
     </row>
-    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="6"/>
     </row>
-    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="6"/>
     </row>
-    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="6"/>
     </row>
-    <row r="204" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="6"/>
     </row>
-    <row r="205" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="6"/>
     </row>
-    <row r="206" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="6"/>
     </row>
-    <row r="207" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="6"/>
     </row>
-    <row r="208" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="6"/>
     </row>
-    <row r="209" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="6"/>
     </row>
-    <row r="210" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="6"/>
     </row>
-    <row r="211" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="6"/>
     </row>
-    <row r="212" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="6"/>
     </row>
-    <row r="213" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="6"/>
     </row>
-    <row r="214" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="6"/>
     </row>
-    <row r="215" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="6"/>
     </row>
-    <row r="216" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="6"/>
     </row>
-    <row r="217" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="6"/>
     </row>
-    <row r="218" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="6"/>
     </row>
-    <row r="219" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="6"/>
     </row>
-    <row r="220" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="6"/>
     </row>
-    <row r="221" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="6"/>
     </row>
-    <row r="222" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="6"/>
     </row>
-    <row r="223" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="6"/>
     </row>
-    <row r="224" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="6"/>
     </row>
-    <row r="225" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="6"/>
     </row>
-    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="6"/>
     </row>
-    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="6"/>
     </row>
-    <row r="228" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="6"/>
     </row>
-    <row r="229" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="6"/>
     </row>
-    <row r="230" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
     </row>
-    <row r="231" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="6"/>
     </row>
-    <row r="232" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="6"/>
     </row>
-    <row r="233" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="6"/>
     </row>
-    <row r="234" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="6"/>
     </row>
-    <row r="235" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="6"/>
     </row>
-    <row r="236" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="6"/>
     </row>
-    <row r="237" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="6"/>
     </row>
-    <row r="238" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="6"/>
     </row>
-    <row r="239" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="6"/>
     </row>
-    <row r="240" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="6"/>
     </row>
-    <row r="241" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="6"/>
     </row>
-    <row r="242" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="6"/>
     </row>
-    <row r="243" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="6"/>
     </row>
-    <row r="244" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="6"/>
     </row>
-    <row r="245" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="6"/>
     </row>
-    <row r="246" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="6"/>
     </row>
-    <row r="247" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="6"/>
     </row>
-    <row r="248" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="6"/>
     </row>
-    <row r="249" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="6"/>
     </row>
-    <row r="250" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="6"/>
     </row>
-    <row r="251" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="6"/>
     </row>
-    <row r="252" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="6"/>
     </row>
-    <row r="253" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="6"/>
     </row>
-    <row r="254" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="6"/>
     </row>
-    <row r="255" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="6"/>
     </row>
-    <row r="256" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="6"/>
     </row>
-    <row r="257" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="6"/>
     </row>
-    <row r="258" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="6"/>
     </row>
-    <row r="259" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="6"/>
     </row>
-    <row r="260" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="6"/>
     </row>
-    <row r="261" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="6"/>
     </row>
-    <row r="262" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="6"/>
     </row>
-    <row r="263" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="6"/>
     </row>
-    <row r="264" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="6"/>
     </row>
-    <row r="265" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="6"/>
     </row>
-    <row r="266" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="6"/>
     </row>
-    <row r="267" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="6"/>
     </row>
-    <row r="268" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="6"/>
     </row>
-    <row r="269" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" s="6"/>
     </row>
-    <row r="270" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="6"/>
     </row>
-    <row r="271" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="6"/>
     </row>
-    <row r="272" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="6"/>
     </row>
-    <row r="273" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="6"/>
     </row>
-    <row r="274" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="6"/>
     </row>
-    <row r="275" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="6"/>
     </row>
-    <row r="276" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="6"/>
     </row>
-    <row r="277" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="6"/>
     </row>
-    <row r="278" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="6"/>
     </row>
-    <row r="279" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="6"/>
     </row>
-    <row r="280" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="6"/>
     </row>
-    <row r="281" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="6"/>
     </row>
-    <row r="282" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="6"/>
     </row>
-    <row r="283" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="6"/>
     </row>
-    <row r="284" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="6"/>
     </row>
-    <row r="285" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="6"/>
     </row>
-    <row r="286" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="6"/>
     </row>
-    <row r="287" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="6"/>
     </row>
-    <row r="288" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="6"/>
     </row>
-    <row r="289" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="6"/>
     </row>
-    <row r="290" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="6"/>
     </row>
-    <row r="291" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="6"/>
     </row>
-    <row r="292" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="6"/>
     </row>
-    <row r="293" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="6"/>
     </row>
-    <row r="294" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="6"/>
     </row>
-    <row r="295" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="6"/>
     </row>
-    <row r="296" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="6"/>
     </row>
-    <row r="297" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="6"/>
     </row>
-    <row r="298" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="6"/>
     </row>
-    <row r="299" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="6"/>
     </row>
-    <row r="300" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="6"/>
     </row>
-    <row r="301" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="6"/>
     </row>
-    <row r="302" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="6"/>
     </row>
-    <row r="303" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="6"/>
     </row>
-    <row r="304" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="6"/>
     </row>
-    <row r="305" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="6"/>
     </row>
-    <row r="306" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="6"/>
     </row>
-    <row r="307" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" s="6"/>
     </row>
-    <row r="308" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="6"/>
     </row>
-    <row r="309" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="6"/>
     </row>
-    <row r="310" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="6"/>
     </row>
-    <row r="311" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" s="6"/>
     </row>
-    <row r="312" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="6"/>
     </row>
-    <row r="313" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="6"/>
     </row>
-    <row r="314" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="6"/>
     </row>
-    <row r="315" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="6"/>
     </row>
-    <row r="316" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="6"/>
     </row>
-    <row r="317" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" s="6"/>
     </row>
-    <row r="318" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="6"/>
     </row>
-    <row r="319" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="6"/>
     </row>
-    <row r="320" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" s="6"/>
     </row>
-    <row r="321" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="6"/>
     </row>
-    <row r="322" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="6"/>
     </row>
-    <row r="323" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" s="6"/>
     </row>
-    <row r="324" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="6"/>
     </row>
-    <row r="325" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="6"/>
     </row>
-    <row r="326" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="6"/>
     </row>
-    <row r="327" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="6"/>
     </row>
-    <row r="328" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="6"/>
     </row>
-    <row r="329" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="6"/>
     </row>
-    <row r="330" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="6"/>
     </row>
-    <row r="331" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" s="6"/>
     </row>
-    <row r="332" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="6"/>
     </row>
-    <row r="333" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="6"/>
     </row>
-    <row r="334" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="6"/>
     </row>
-    <row r="335" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="6"/>
     </row>
-    <row r="336" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="6"/>
     </row>
-    <row r="337" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="6"/>
     </row>
-    <row r="338" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="6"/>
     </row>
-    <row r="339" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" s="6"/>
     </row>
-    <row r="340" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="6"/>
     </row>
-    <row r="341" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="6"/>
     </row>
-    <row r="342" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="6"/>
     </row>
-    <row r="343" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" s="6"/>
     </row>
-    <row r="344" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="6"/>
     </row>
-    <row r="345" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="6"/>
     </row>
-    <row r="346" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="6"/>
     </row>
-    <row r="347" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="6"/>
     </row>
-    <row r="348" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" s="6"/>
     </row>
-    <row r="349" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="6"/>
     </row>
-    <row r="350" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="6"/>
     </row>
-    <row r="351" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="6"/>
     </row>
-    <row r="352" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="6"/>
     </row>
-    <row r="353" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="6"/>
     </row>
-    <row r="354" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" s="6"/>
     </row>
-    <row r="355" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="6"/>
     </row>
-    <row r="356" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" s="6"/>
     </row>
-    <row r="357" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="6"/>
     </row>
-    <row r="358" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="6"/>
     </row>
-    <row r="359" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="6"/>
     </row>
-    <row r="360" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="6"/>
     </row>
-    <row r="361" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="6"/>
     </row>
-    <row r="362" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="6"/>
     </row>
-    <row r="363" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="6"/>
     </row>
-    <row r="364" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="6"/>
     </row>
-    <row r="365" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="6"/>
     </row>
-    <row r="366" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="6"/>
     </row>
-    <row r="367" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" s="6"/>
     </row>
-    <row r="368" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="6"/>
     </row>
-    <row r="369" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" s="6"/>
     </row>
-    <row r="370" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="6"/>
     </row>
-    <row r="371" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="6"/>
     </row>
-    <row r="372" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="6"/>
     </row>
-    <row r="373" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="6"/>
     </row>
-    <row r="374" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="6"/>
     </row>
-    <row r="375" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="6"/>
     </row>
-    <row r="376" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="6"/>
     </row>
-    <row r="377" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="6"/>
     </row>
-    <row r="378" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" s="6"/>
     </row>
-    <row r="379" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="6"/>
     </row>
-    <row r="380" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="6"/>
     </row>
-    <row r="381" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="6"/>
     </row>
-    <row r="382" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="6"/>
     </row>
-    <row r="383" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" s="6"/>
     </row>
-    <row r="384" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" s="6"/>
     </row>
-    <row r="385" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="6"/>
     </row>
-    <row r="386" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="6"/>
     </row>
-    <row r="387" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="6"/>
     </row>
-    <row r="388" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="6"/>
     </row>
-    <row r="389" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="6"/>
     </row>
-    <row r="390" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="6"/>
     </row>
-    <row r="391" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="6"/>
     </row>
-    <row r="392" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="6"/>
     </row>
-    <row r="393" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" s="6"/>
     </row>
-    <row r="394" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="6"/>
     </row>
-    <row r="395" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="6"/>
     </row>
-    <row r="396" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" s="6"/>
     </row>
-    <row r="397" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="6"/>
     </row>
-    <row r="398" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="6"/>
     </row>
-    <row r="399" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" s="6"/>
     </row>
-    <row r="400" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="6"/>
     </row>
-    <row r="401" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="6"/>
     </row>
-    <row r="402" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="6"/>
     </row>
-    <row r="403" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="6"/>
     </row>
-    <row r="404" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="6"/>
     </row>
-    <row r="405" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="6"/>
     </row>
-    <row r="406" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="6"/>
     </row>
-    <row r="407" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="6"/>
     </row>
-    <row r="408" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" s="6"/>
     </row>
-    <row r="409" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" s="6"/>
     </row>
-    <row r="410" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="6"/>
     </row>
-    <row r="411" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="6"/>
     </row>
-    <row r="412" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="6"/>
     </row>
-    <row r="413" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="6"/>
     </row>
-    <row r="414" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" s="6"/>
     </row>
-    <row r="415" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="6"/>
     </row>
-    <row r="416" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="6"/>
     </row>
-    <row r="417" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="6"/>
     </row>
-    <row r="418" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="6"/>
     </row>
-    <row r="419" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="6"/>
     </row>
-    <row r="420" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="6"/>
     </row>
-    <row r="421" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421" s="6"/>
     </row>
-    <row r="422" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="6"/>
     </row>
-    <row r="423" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423" s="6"/>
     </row>
-    <row r="424" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="6"/>
     </row>
-    <row r="425" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="6"/>
     </row>
-    <row r="426" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="6"/>
     </row>
-    <row r="427" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="6"/>
     </row>
-    <row r="428" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="6"/>
     </row>
-    <row r="429" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429" s="6"/>
     </row>
-    <row r="430" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="6"/>
     </row>
-    <row r="431" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="6"/>
     </row>
-    <row r="432" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="6"/>
     </row>
-    <row r="433" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="6"/>
     </row>
-    <row r="434" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434" s="6"/>
     </row>
-    <row r="435" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="6"/>
     </row>
-    <row r="436" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="6"/>
     </row>
-    <row r="437" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="6"/>
     </row>
-    <row r="438" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438" s="6"/>
     </row>
-    <row r="439" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="6"/>
     </row>
-    <row r="440" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="6"/>
     </row>
-    <row r="441" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="6"/>
     </row>
-    <row r="442" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="6"/>
     </row>
-    <row r="443" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="6"/>
     </row>
-    <row r="444" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444" s="6"/>
     </row>
-    <row r="445" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="6"/>
     </row>
-    <row r="446" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="6"/>
     </row>
-    <row r="447" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="6"/>
     </row>
-    <row r="448" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="6"/>
     </row>
-    <row r="449" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="6"/>
     </row>
-    <row r="450" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="6"/>
     </row>
-    <row r="451" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="6"/>
     </row>
-    <row r="452" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="6"/>
     </row>
-    <row r="453" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453" s="6"/>
     </row>
-    <row r="454" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454" s="6"/>
     </row>
-    <row r="455" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="6"/>
     </row>
-    <row r="456" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456" s="6"/>
     </row>
-    <row r="457" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457" s="6"/>
     </row>
-    <row r="458" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="6"/>
     </row>
-    <row r="459" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459" s="6"/>
     </row>
-    <row r="460" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A460" s="6"/>
     </row>
-    <row r="461" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461" s="6"/>
     </row>
-    <row r="462" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462" s="6"/>
     </row>
-    <row r="463" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463" s="6"/>
     </row>
-    <row r="464" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464" s="6"/>
     </row>
-    <row r="465" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465" s="6"/>
     </row>
-    <row r="466" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466" s="6"/>
     </row>
-    <row r="467" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467" s="6"/>
     </row>
-    <row r="468" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A468" s="6"/>
     </row>
-    <row r="469" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469" s="6"/>
     </row>
-    <row r="470" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470" s="6"/>
     </row>
-    <row r="471" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="6"/>
     </row>
-    <row r="472" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="6"/>
     </row>
-    <row r="473" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473" s="6"/>
     </row>
-    <row r="474" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474" s="6"/>
     </row>
-    <row r="475" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475" s="6"/>
     </row>
-    <row r="476" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A476" s="6"/>
     </row>
-    <row r="477" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477" s="6"/>
     </row>
-    <row r="478" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478" s="6"/>
     </row>
-    <row r="479" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479" s="6"/>
     </row>
-    <row r="480" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480" s="6"/>
     </row>
-    <row r="481" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481" s="6"/>
     </row>
-    <row r="482" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="6"/>
     </row>
-    <row r="483" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483" s="6"/>
     </row>
-    <row r="484" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484" s="6"/>
     </row>
-    <row r="485" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485" s="6"/>
     </row>
-    <row r="486" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486" s="6"/>
     </row>
-    <row r="487" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487" s="6"/>
     </row>
-    <row r="488" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488" s="6"/>
     </row>
-    <row r="489" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489" s="6"/>
     </row>
-    <row r="490" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490" s="6"/>
     </row>
-    <row r="491" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491" s="6"/>
     </row>
-    <row r="492" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492" s="6"/>
     </row>
-    <row r="493" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493" s="6"/>
     </row>
-    <row r="494" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494" s="6"/>
     </row>
-    <row r="495" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495" s="6"/>
     </row>
-    <row r="496" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496" s="6"/>
     </row>
-    <row r="497" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497" s="6"/>
     </row>
-    <row r="498" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498" s="6"/>
     </row>
-    <row r="499" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499" s="6"/>
     </row>
-    <row r="500" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500" s="6"/>
     </row>
-    <row r="501" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501" s="6"/>
     </row>
-    <row r="502" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502" s="6"/>
     </row>
   </sheetData>
@@ -2360,25 +2441,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="3"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="3"/>
+    <col min="1" max="1" width="16.5546875" style="3"/>
+    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="16.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2392,7 +2475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>44</v>
@@ -2404,7 +2487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2418,7 +2501,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2432,7 +2515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2446,7 +2529,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -2460,7 +2543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -2474,7 +2557,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2488,7 +2571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2502,7 +2585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -2516,7 +2599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -2530,7 +2613,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2544,7 +2627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2558,7 +2641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2572,7 +2655,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -2586,7 +2669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -2600,7 +2683,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -2614,7 +2697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -2628,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>38</v>
@@ -2640,7 +2723,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>52</v>
@@ -2652,7 +2735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>53</v>
@@ -2664,7 +2747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>39</v>
@@ -2676,7 +2759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>20</v>
@@ -2688,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>21</v>
@@ -2700,7 +2783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>48</v>
@@ -2712,7 +2795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>22</v>
@@ -2724,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>23</v>
@@ -2736,7 +2819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>24</v>
@@ -2748,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>49</v>
@@ -2760,7 +2843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>25</v>
@@ -2772,7 +2855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>9</v>
@@ -2784,7 +2867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>26</v>
@@ -2796,7 +2879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>28</v>
@@ -2808,7 +2891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>29</v>
@@ -2820,7 +2903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>30</v>
@@ -2832,7 +2915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>31</v>
@@ -2844,7 +2927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>32</v>
@@ -2856,7 +2939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>75</v>
@@ -2868,7 +2951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
         <v>10</v>
@@ -2880,7 +2963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
         <v>34</v>
@@ -2892,7 +2975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
         <v>35</v>
@@ -2904,15 +2987,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="7">
+        <v>41</v>
+      </c>
+      <c r="D43" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="4">
-        <v>41</v>
-      </c>
-      <c r="D43" s="4"/>
+      <c r="C44" s="7">
+        <v>42</v>
+      </c>
+      <c r="D44" s="7">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CREATCMR-5718 mod massUpd template
CREATCMR-5718 mod massUpd template
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateUS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateUS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADBB471-51AC-42E5-9CDE-3E0675886B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F119ED9-3C52-4F7B-9FD6-0A2D8BCBC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>MKTG_DEPT</t>
   </si>
   <si>
-    <t>ISU_CD</t>
-  </si>
-  <si>
     <t>ZS01</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>ISIC Code</t>
   </si>
   <si>
-    <t>OUT_CITY_LIMIT</t>
-  </si>
-  <si>
     <t>PCC_AR_DEPT</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>CSO_SITE</t>
   </si>
   <si>
-    <t>MISC_BILL_CD</t>
-  </si>
-  <si>
     <t>Abbreviated Name</t>
   </si>
   <si>
@@ -122,12 +113,6 @@
     <t>TAX_CD3</t>
   </si>
   <si>
-    <t>ISU Code</t>
-  </si>
-  <si>
-    <t>INAC_CD</t>
-  </si>
-  <si>
     <t>CLIENT_TIER</t>
   </si>
   <si>
@@ -185,9 +170,6 @@
     <t>CUST_NM2</t>
   </si>
   <si>
-    <t>Out of City Limits?</t>
-  </si>
-  <si>
     <t>PCC AR Dept.</t>
   </si>
   <si>
@@ -212,9 +194,6 @@
     <t>Marketing Dept.</t>
   </si>
   <si>
-    <t>Misc Bill Code</t>
-  </si>
-  <si>
     <t>ICC Tax Class</t>
   </si>
   <si>
@@ -230,9 +209,6 @@
     <t>Tax Class / Code 3</t>
   </si>
   <si>
-    <t>INAC Code</t>
-  </si>
-  <si>
     <t>Client Tier</t>
   </si>
   <si>
@@ -243,18 +219,6 @@
   </si>
   <si>
     <t>County</t>
-  </si>
-  <si>
-    <t>Enterprise</t>
-  </si>
-  <si>
-    <t>ENTERPRISE</t>
-  </si>
-  <si>
-    <t>Tax Exempt Status</t>
-  </si>
-  <si>
-    <t>TAX_EXEMPT_STATUS_1</t>
   </si>
   <si>
     <t>Search Term</t>
@@ -280,18 +244,6 @@
     <t>COMPANY</t>
   </si>
   <si>
-    <t>Tax Exempt Status2</t>
-  </si>
-  <si>
-    <t>Tax Exempt Status3</t>
-  </si>
-  <si>
-    <t>TAX_EXEMPT_STATUS_2</t>
-  </si>
-  <si>
-    <t>TAX_EXEMPT_STATUS_3</t>
-  </si>
-  <si>
     <t>Order Block code</t>
   </si>
   <si>
@@ -300,6 +252,70 @@
   </si>
   <si>
     <t>EDUC_ALLOW_CD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>OUT_CITY_LIMIT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>MISC_BILL_CD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Out of City Limits?</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Misc Bill Code</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TAX_EXEMPT_STATUS_1</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ENTERPRISE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Enterprise</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Tax Exempt Status</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ISU_CD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TAX_EXEMPT_STATUS_2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>INAC_CD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TAX_EXEMPT_STATUS_3</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Tax Exempt Status2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ISU Code</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Tax Exempt Status3</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>INAC Code</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -307,11 +323,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -319,7 +335,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -327,7 +343,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -336,24 +352,30 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -368,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -389,12 +411,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -706,59 +740,63 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AW502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.4140625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="20.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="7" width="20.4140625" style="10"/>
+    <col min="31" max="39" width="20.4140625" style="10"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="3" customFormat="1">
+    <row r="1" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -773,15 +811,15 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
@@ -792,10 +830,10 @@
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" s="3" customFormat="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,22 +844,22 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
@@ -830,1618 +868,1618 @@
         <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AL2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="AW2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="6"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="6"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="6"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="6"/>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="6"/>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="6"/>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="6"/>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="6"/>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="6"/>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="6"/>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="6"/>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="6"/>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="6"/>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="6"/>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="6"/>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="6"/>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="6"/>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="6"/>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="6"/>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="6"/>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="6"/>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="6"/>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="6"/>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="6"/>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="6"/>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="6"/>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="6"/>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="6"/>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="6"/>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="6"/>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="6"/>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="6"/>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="6"/>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="6"/>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="6"/>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="6"/>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="6"/>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="6"/>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="6"/>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="6"/>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="6"/>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="6"/>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="6"/>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="6"/>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="6"/>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="6"/>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="6"/>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="6"/>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="6"/>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="6"/>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="6"/>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="6"/>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="6"/>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="6"/>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="6"/>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="6"/>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="6"/>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="6"/>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="6"/>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="6"/>
     </row>
-    <row r="239" spans="1:1">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="6"/>
     </row>
-    <row r="240" spans="1:1">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="6"/>
     </row>
-    <row r="241" spans="1:1">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="6"/>
     </row>
-    <row r="242" spans="1:1">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="6"/>
     </row>
-    <row r="243" spans="1:1">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="6"/>
     </row>
-    <row r="244" spans="1:1">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="6"/>
     </row>
-    <row r="245" spans="1:1">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="6"/>
     </row>
-    <row r="246" spans="1:1">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="6"/>
     </row>
-    <row r="247" spans="1:1">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="6"/>
     </row>
-    <row r="248" spans="1:1">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="6"/>
     </row>
-    <row r="249" spans="1:1">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="6"/>
     </row>
-    <row r="250" spans="1:1">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="6"/>
     </row>
-    <row r="251" spans="1:1">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="6"/>
     </row>
-    <row r="252" spans="1:1">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="6"/>
     </row>
-    <row r="253" spans="1:1">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="6"/>
     </row>
-    <row r="254" spans="1:1">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="6"/>
     </row>
-    <row r="255" spans="1:1">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="6"/>
     </row>
-    <row r="256" spans="1:1">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="6"/>
     </row>
-    <row r="257" spans="1:1">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="6"/>
     </row>
-    <row r="258" spans="1:1">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="6"/>
     </row>
-    <row r="259" spans="1:1">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="6"/>
     </row>
-    <row r="260" spans="1:1">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="6"/>
     </row>
-    <row r="261" spans="1:1">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="6"/>
     </row>
-    <row r="262" spans="1:1">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="6"/>
     </row>
-    <row r="263" spans="1:1">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="6"/>
     </row>
-    <row r="264" spans="1:1">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="6"/>
     </row>
-    <row r="265" spans="1:1">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="6"/>
     </row>
-    <row r="266" spans="1:1">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="6"/>
     </row>
-    <row r="267" spans="1:1">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="6"/>
     </row>
-    <row r="268" spans="1:1">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="6"/>
     </row>
-    <row r="269" spans="1:1">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" s="6"/>
     </row>
-    <row r="270" spans="1:1">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="6"/>
     </row>
-    <row r="271" spans="1:1">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="6"/>
     </row>
-    <row r="272" spans="1:1">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="6"/>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="6"/>
     </row>
-    <row r="274" spans="1:1">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="6"/>
     </row>
-    <row r="275" spans="1:1">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="6"/>
     </row>
-    <row r="276" spans="1:1">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="6"/>
     </row>
-    <row r="277" spans="1:1">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="6"/>
     </row>
-    <row r="278" spans="1:1">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="6"/>
     </row>
-    <row r="279" spans="1:1">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="6"/>
     </row>
-    <row r="280" spans="1:1">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="6"/>
     </row>
-    <row r="281" spans="1:1">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="6"/>
     </row>
-    <row r="282" spans="1:1">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="6"/>
     </row>
-    <row r="283" spans="1:1">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="6"/>
     </row>
-    <row r="284" spans="1:1">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="6"/>
     </row>
-    <row r="285" spans="1:1">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="6"/>
     </row>
-    <row r="286" spans="1:1">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="6"/>
     </row>
-    <row r="287" spans="1:1">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="6"/>
     </row>
-    <row r="288" spans="1:1">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="6"/>
     </row>
-    <row r="289" spans="1:1">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="6"/>
     </row>
-    <row r="290" spans="1:1">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="6"/>
     </row>
-    <row r="291" spans="1:1">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="6"/>
     </row>
-    <row r="292" spans="1:1">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="6"/>
     </row>
-    <row r="293" spans="1:1">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="6"/>
     </row>
-    <row r="294" spans="1:1">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="6"/>
     </row>
-    <row r="295" spans="1:1">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="6"/>
     </row>
-    <row r="296" spans="1:1">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="6"/>
     </row>
-    <row r="297" spans="1:1">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="6"/>
     </row>
-    <row r="298" spans="1:1">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="6"/>
     </row>
-    <row r="299" spans="1:1">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="6"/>
     </row>
-    <row r="300" spans="1:1">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="6"/>
     </row>
-    <row r="301" spans="1:1">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="6"/>
     </row>
-    <row r="302" spans="1:1">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="6"/>
     </row>
-    <row r="303" spans="1:1">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="6"/>
     </row>
-    <row r="304" spans="1:1">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="6"/>
     </row>
-    <row r="305" spans="1:1">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="6"/>
     </row>
-    <row r="306" spans="1:1">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="6"/>
     </row>
-    <row r="307" spans="1:1">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" s="6"/>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="6"/>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="6"/>
     </row>
-    <row r="310" spans="1:1">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="6"/>
     </row>
-    <row r="311" spans="1:1">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" s="6"/>
     </row>
-    <row r="312" spans="1:1">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="6"/>
     </row>
-    <row r="313" spans="1:1">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="6"/>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="6"/>
     </row>
-    <row r="315" spans="1:1">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="6"/>
     </row>
-    <row r="316" spans="1:1">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="6"/>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" s="6"/>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="6"/>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="6"/>
     </row>
-    <row r="320" spans="1:1">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" s="6"/>
     </row>
-    <row r="321" spans="1:1">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="6"/>
     </row>
-    <row r="322" spans="1:1">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="6"/>
     </row>
-    <row r="323" spans="1:1">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" s="6"/>
     </row>
-    <row r="324" spans="1:1">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="6"/>
     </row>
-    <row r="325" spans="1:1">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="6"/>
     </row>
-    <row r="326" spans="1:1">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="6"/>
     </row>
-    <row r="327" spans="1:1">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="6"/>
     </row>
-    <row r="328" spans="1:1">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="6"/>
     </row>
-    <row r="329" spans="1:1">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="6"/>
     </row>
-    <row r="330" spans="1:1">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="6"/>
     </row>
-    <row r="331" spans="1:1">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" s="6"/>
     </row>
-    <row r="332" spans="1:1">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="6"/>
     </row>
-    <row r="333" spans="1:1">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="6"/>
     </row>
-    <row r="334" spans="1:1">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="6"/>
     </row>
-    <row r="335" spans="1:1">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="6"/>
     </row>
-    <row r="336" spans="1:1">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="6"/>
     </row>
-    <row r="337" spans="1:1">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="6"/>
     </row>
-    <row r="338" spans="1:1">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="6"/>
     </row>
-    <row r="339" spans="1:1">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" s="6"/>
     </row>
-    <row r="340" spans="1:1">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="6"/>
     </row>
-    <row r="341" spans="1:1">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="6"/>
     </row>
-    <row r="342" spans="1:1">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="6"/>
     </row>
-    <row r="343" spans="1:1">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" s="6"/>
     </row>
-    <row r="344" spans="1:1">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="6"/>
     </row>
-    <row r="345" spans="1:1">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="6"/>
     </row>
-    <row r="346" spans="1:1">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="6"/>
     </row>
-    <row r="347" spans="1:1">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="6"/>
     </row>
-    <row r="348" spans="1:1">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" s="6"/>
     </row>
-    <row r="349" spans="1:1">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="6"/>
     </row>
-    <row r="350" spans="1:1">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="6"/>
     </row>
-    <row r="351" spans="1:1">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="6"/>
     </row>
-    <row r="352" spans="1:1">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="6"/>
     </row>
-    <row r="353" spans="1:1">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="6"/>
     </row>
-    <row r="354" spans="1:1">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" s="6"/>
     </row>
-    <row r="355" spans="1:1">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="6"/>
     </row>
-    <row r="356" spans="1:1">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" s="6"/>
     </row>
-    <row r="357" spans="1:1">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="6"/>
     </row>
-    <row r="358" spans="1:1">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="6"/>
     </row>
-    <row r="359" spans="1:1">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="6"/>
     </row>
-    <row r="360" spans="1:1">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="6"/>
     </row>
-    <row r="361" spans="1:1">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="6"/>
     </row>
-    <row r="362" spans="1:1">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="6"/>
     </row>
-    <row r="363" spans="1:1">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="6"/>
     </row>
-    <row r="364" spans="1:1">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="6"/>
     </row>
-    <row r="365" spans="1:1">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="6"/>
     </row>
-    <row r="366" spans="1:1">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="6"/>
     </row>
-    <row r="367" spans="1:1">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" s="6"/>
     </row>
-    <row r="368" spans="1:1">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="6"/>
     </row>
-    <row r="369" spans="1:1">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" s="6"/>
     </row>
-    <row r="370" spans="1:1">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="6"/>
     </row>
-    <row r="371" spans="1:1">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="6"/>
     </row>
-    <row r="372" spans="1:1">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="6"/>
     </row>
-    <row r="373" spans="1:1">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="6"/>
     </row>
-    <row r="374" spans="1:1">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="6"/>
     </row>
-    <row r="375" spans="1:1">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="6"/>
     </row>
-    <row r="376" spans="1:1">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="6"/>
     </row>
-    <row r="377" spans="1:1">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="6"/>
     </row>
-    <row r="378" spans="1:1">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" s="6"/>
     </row>
-    <row r="379" spans="1:1">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="6"/>
     </row>
-    <row r="380" spans="1:1">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="6"/>
     </row>
-    <row r="381" spans="1:1">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="6"/>
     </row>
-    <row r="382" spans="1:1">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="6"/>
     </row>
-    <row r="383" spans="1:1">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" s="6"/>
     </row>
-    <row r="384" spans="1:1">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" s="6"/>
     </row>
-    <row r="385" spans="1:1">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="6"/>
     </row>
-    <row r="386" spans="1:1">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="6"/>
     </row>
-    <row r="387" spans="1:1">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="6"/>
     </row>
-    <row r="388" spans="1:1">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="6"/>
     </row>
-    <row r="389" spans="1:1">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="6"/>
     </row>
-    <row r="390" spans="1:1">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="6"/>
     </row>
-    <row r="391" spans="1:1">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="6"/>
     </row>
-    <row r="392" spans="1:1">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="6"/>
     </row>
-    <row r="393" spans="1:1">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" s="6"/>
     </row>
-    <row r="394" spans="1:1">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="6"/>
     </row>
-    <row r="395" spans="1:1">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="6"/>
     </row>
-    <row r="396" spans="1:1">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" s="6"/>
     </row>
-    <row r="397" spans="1:1">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="6"/>
     </row>
-    <row r="398" spans="1:1">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="6"/>
     </row>
-    <row r="399" spans="1:1">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" s="6"/>
     </row>
-    <row r="400" spans="1:1">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="6"/>
     </row>
-    <row r="401" spans="1:1">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="6"/>
     </row>
-    <row r="402" spans="1:1">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="6"/>
     </row>
-    <row r="403" spans="1:1">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="6"/>
     </row>
-    <row r="404" spans="1:1">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="6"/>
     </row>
-    <row r="405" spans="1:1">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="6"/>
     </row>
-    <row r="406" spans="1:1">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="6"/>
     </row>
-    <row r="407" spans="1:1">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="6"/>
     </row>
-    <row r="408" spans="1:1">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" s="6"/>
     </row>
-    <row r="409" spans="1:1">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" s="6"/>
     </row>
-    <row r="410" spans="1:1">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="6"/>
     </row>
-    <row r="411" spans="1:1">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="6"/>
     </row>
-    <row r="412" spans="1:1">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="6"/>
     </row>
-    <row r="413" spans="1:1">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="6"/>
     </row>
-    <row r="414" spans="1:1">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" s="6"/>
     </row>
-    <row r="415" spans="1:1">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="6"/>
     </row>
-    <row r="416" spans="1:1">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="6"/>
     </row>
-    <row r="417" spans="1:1">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="6"/>
     </row>
-    <row r="418" spans="1:1">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="6"/>
     </row>
-    <row r="419" spans="1:1">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="6"/>
     </row>
-    <row r="420" spans="1:1">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="6"/>
     </row>
-    <row r="421" spans="1:1">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421" s="6"/>
     </row>
-    <row r="422" spans="1:1">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="6"/>
     </row>
-    <row r="423" spans="1:1">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423" s="6"/>
     </row>
-    <row r="424" spans="1:1">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="6"/>
     </row>
-    <row r="425" spans="1:1">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="6"/>
     </row>
-    <row r="426" spans="1:1">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="6"/>
     </row>
-    <row r="427" spans="1:1">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="6"/>
     </row>
-    <row r="428" spans="1:1">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="6"/>
     </row>
-    <row r="429" spans="1:1">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429" s="6"/>
     </row>
-    <row r="430" spans="1:1">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="6"/>
     </row>
-    <row r="431" spans="1:1">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="6"/>
     </row>
-    <row r="432" spans="1:1">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="6"/>
     </row>
-    <row r="433" spans="1:1">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="6"/>
     </row>
-    <row r="434" spans="1:1">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434" s="6"/>
     </row>
-    <row r="435" spans="1:1">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="6"/>
     </row>
-    <row r="436" spans="1:1">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="6"/>
     </row>
-    <row r="437" spans="1:1">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="6"/>
     </row>
-    <row r="438" spans="1:1">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438" s="6"/>
     </row>
-    <row r="439" spans="1:1">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="6"/>
     </row>
-    <row r="440" spans="1:1">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="6"/>
     </row>
-    <row r="441" spans="1:1">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="6"/>
     </row>
-    <row r="442" spans="1:1">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="6"/>
     </row>
-    <row r="443" spans="1:1">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="6"/>
     </row>
-    <row r="444" spans="1:1">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444" s="6"/>
     </row>
-    <row r="445" spans="1:1">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="6"/>
     </row>
-    <row r="446" spans="1:1">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="6"/>
     </row>
-    <row r="447" spans="1:1">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="6"/>
     </row>
-    <row r="448" spans="1:1">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="6"/>
     </row>
-    <row r="449" spans="1:1">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="6"/>
     </row>
-    <row r="450" spans="1:1">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="6"/>
     </row>
-    <row r="451" spans="1:1">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="6"/>
     </row>
-    <row r="452" spans="1:1">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="6"/>
     </row>
-    <row r="453" spans="1:1">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453" s="6"/>
     </row>
-    <row r="454" spans="1:1">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454" s="6"/>
     </row>
-    <row r="455" spans="1:1">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="6"/>
     </row>
-    <row r="456" spans="1:1">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456" s="6"/>
     </row>
-    <row r="457" spans="1:1">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457" s="6"/>
     </row>
-    <row r="458" spans="1:1">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="6"/>
     </row>
-    <row r="459" spans="1:1">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459" s="6"/>
     </row>
-    <row r="460" spans="1:1">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A460" s="6"/>
     </row>
-    <row r="461" spans="1:1">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461" s="6"/>
     </row>
-    <row r="462" spans="1:1">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462" s="6"/>
     </row>
-    <row r="463" spans="1:1">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463" s="6"/>
     </row>
-    <row r="464" spans="1:1">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464" s="6"/>
     </row>
-    <row r="465" spans="1:1">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465" s="6"/>
     </row>
-    <row r="466" spans="1:1">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466" s="6"/>
     </row>
-    <row r="467" spans="1:1">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467" s="6"/>
     </row>
-    <row r="468" spans="1:1">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A468" s="6"/>
     </row>
-    <row r="469" spans="1:1">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469" s="6"/>
     </row>
-    <row r="470" spans="1:1">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470" s="6"/>
     </row>
-    <row r="471" spans="1:1">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="6"/>
     </row>
-    <row r="472" spans="1:1">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="6"/>
     </row>
-    <row r="473" spans="1:1">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473" s="6"/>
     </row>
-    <row r="474" spans="1:1">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474" s="6"/>
     </row>
-    <row r="475" spans="1:1">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475" s="6"/>
     </row>
-    <row r="476" spans="1:1">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A476" s="6"/>
     </row>
-    <row r="477" spans="1:1">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477" s="6"/>
     </row>
-    <row r="478" spans="1:1">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478" s="6"/>
     </row>
-    <row r="479" spans="1:1">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479" s="6"/>
     </row>
-    <row r="480" spans="1:1">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480" s="6"/>
     </row>
-    <row r="481" spans="1:1">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481" s="6"/>
     </row>
-    <row r="482" spans="1:1">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="6"/>
     </row>
-    <row r="483" spans="1:1">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483" s="6"/>
     </row>
-    <row r="484" spans="1:1">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484" s="6"/>
     </row>
-    <row r="485" spans="1:1">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485" s="6"/>
     </row>
-    <row r="486" spans="1:1">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486" s="6"/>
     </row>
-    <row r="487" spans="1:1">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487" s="6"/>
     </row>
-    <row r="488" spans="1:1">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488" s="6"/>
     </row>
-    <row r="489" spans="1:1">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489" s="6"/>
     </row>
-    <row r="490" spans="1:1">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490" s="6"/>
     </row>
-    <row r="491" spans="1:1">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491" s="6"/>
     </row>
-    <row r="492" spans="1:1">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492" s="6"/>
     </row>
-    <row r="493" spans="1:1">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493" s="6"/>
     </row>
-    <row r="494" spans="1:1">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494" s="6"/>
     </row>
-    <row r="495" spans="1:1">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495" s="6"/>
     </row>
-    <row r="496" spans="1:1">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496" s="6"/>
     </row>
-    <row r="497" spans="1:1">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497" s="6"/>
     </row>
-    <row r="498" spans="1:1">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498" s="6"/>
     </row>
-    <row r="499" spans="1:1">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499" s="6"/>
     </row>
-    <row r="500" spans="1:1">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500" s="6"/>
     </row>
-    <row r="501" spans="1:1">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501" s="6"/>
     </row>
-    <row r="502" spans="1:1">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502" s="6"/>
     </row>
   </sheetData>
@@ -2463,19 +2501,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.58203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="16.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.58203125" style="3"/>
     <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
     <col min="3" max="16384" width="16.58203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2486,13 +2524,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -2501,9 +2539,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -2515,9 +2553,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -2529,12 +2567,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -2543,12 +2581,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
         <v>5</v>
@@ -2557,12 +2595,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4">
         <v>6</v>
@@ -2571,12 +2609,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C9" s="4">
         <v>7</v>
@@ -2585,12 +2623,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4">
         <v>8</v>
@@ -2599,12 +2637,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4">
         <v>9</v>
@@ -2613,9 +2651,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -2627,9 +2665,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
@@ -2641,12 +2679,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4">
         <v>12</v>
@@ -2655,12 +2693,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C15" s="4">
         <v>13</v>
@@ -2669,12 +2707,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4">
         <v>14</v>
@@ -2683,12 +2721,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C17" s="4">
         <v>15</v>
@@ -2697,12 +2735,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4">
         <v>16</v>
@@ -2711,12 +2749,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C19" s="4">
         <v>17</v>
@@ -2725,10 +2763,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4">
         <v>18</v>
@@ -2737,10 +2775,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4">
         <v>19</v>
@@ -2749,10 +2787,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4">
         <v>20</v>
@@ -2761,10 +2799,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4">
         <v>21</v>
@@ -2773,22 +2811,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4">
         <v>22</v>
       </c>
       <c r="D24" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4">
         <v>23</v>
@@ -2797,10 +2835,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C26" s="4">
         <v>24</v>
@@ -2809,10 +2847,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="4">
         <v>25</v>
@@ -2821,10 +2859,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="4">
         <v>26</v>
@@ -2833,10 +2871,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4">
         <v>27</v>
@@ -2845,10 +2883,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C30" s="4">
         <v>28</v>
@@ -2857,10 +2895,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C31" s="4">
         <v>29</v>
@@ -2869,7 +2907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>9</v>
@@ -2881,22 +2919,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C33" s="4">
         <v>31</v>
       </c>
       <c r="D33" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C34" s="4">
         <v>32</v>
@@ -2905,10 +2943,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C35" s="4">
         <v>33</v>
@@ -2917,10 +2955,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C36" s="4">
         <v>34</v>
@@ -2929,10 +2967,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C37" s="4">
         <v>35</v>
@@ -2941,10 +2979,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C38" s="4">
         <v>36</v>
@@ -2953,46 +2991,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C39" s="4">
         <v>37</v>
       </c>
       <c r="D39" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C40" s="4">
         <v>38</v>
       </c>
       <c r="D40" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C41" s="4">
         <v>39</v>
       </c>
       <c r="D41" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4">
         <v>40</v>
@@ -3001,22 +3039,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C43" s="7">
         <v>41</v>
       </c>
       <c r="D43" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C44" s="7">
         <v>42</v>
@@ -3025,10 +3063,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C45" s="7">
         <v>43</v>
@@ -3037,10 +3075,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C46" s="7">
         <v>44</v>
@@ -3049,10 +3087,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C47" s="7">
         <v>45</v>
@@ -3061,34 +3099,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C48" s="7">
         <v>46</v>
       </c>
       <c r="D48" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C49" s="7">
         <v>47</v>
       </c>
       <c r="D49" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C50" s="7">
         <v>48</v>
@@ -3097,10 +3135,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C51" s="7">
         <v>49</v>

</xml_diff>

<commit_message>
CREATCMR-5718 MASSUPD OCL FIX
CREATCMR-5718 MASSUPD OCL FIX
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateUS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateUS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F119ED9-3C52-4F7B-9FD6-0A2D8BCBC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2245C92-0864-4695-A8D5-71F2BD51049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,10 +263,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>Out of City Limits?</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>Misc Bill Code</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -316,6 +312,10 @@
   </si>
   <si>
     <t>INAC Code</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Out of City Limits</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -898,7 +898,7 @@
         <v>18</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>49</v>
@@ -925,7 +925,7 @@
         <v>56</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>57</v>
@@ -943,19 +943,19 @@
         <v>61</v>
       </c>
       <c r="AK2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AL2" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AM2" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>66</v>
@@ -970,10 +970,10 @@
         <v>71</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AV2" s="1" t="s">
         <v>74</v>
@@ -2994,7 +2994,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="4">
         <v>37</v>
@@ -3006,7 +3006,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="4">
         <v>38</v>
@@ -3018,7 +3018,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="4">
         <v>39</v>
@@ -3042,7 +3042,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="7">
         <v>41</v>
@@ -3102,7 +3102,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="7">
         <v>46</v>
@@ -3114,7 +3114,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="7">
         <v>47</v>

</xml_diff>

<commit_message>
CREATCMR-6130 Add BP fields for MassUpd
CREATCMR-6130 Add BP fields for MassUpd
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateUS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateUS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2245C92-0864-4695-A8D5-71F2BD51049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D162F5DE-5331-4E13-BC41-6CFB9617522E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Cmr No.</t>
   </si>
@@ -316,6 +316,109 @@
   </si>
   <si>
     <t>Out of City Limits</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BP Account Type</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Business Partner Name</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BP_ACCT_TYP</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BP_NAME</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BP - BILL-TO / PAYER</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CCR - CAMPUS RESELLER</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>DIS - DISTRIBUTOR</t>
+  </si>
+  <si>
+    <t>FSR - FEDRL SYS RMKT</t>
+  </si>
+  <si>
+    <t>GBR - GENRL BUS RESEL</t>
+  </si>
+  <si>
+    <t>IRMR - IND RMKT MIDRGE</t>
+  </si>
+  <si>
+    <t>IRPC - IND RMKT PC</t>
+  </si>
+  <si>
+    <t>ISV - INDEP S/W VENDR</t>
+  </si>
+  <si>
+    <t>MA - MRKTG ASSISTANT</t>
+  </si>
+  <si>
+    <t>MIR - MANAGING IR</t>
+  </si>
+  <si>
+    <t>PCD - PC DEALER</t>
+  </si>
+  <si>
+    <t>PPR - PSC PRTR RMKT</t>
+  </si>
+  <si>
+    <t>PPS - PSC PRTR SUPL</t>
+  </si>
+  <si>
+    <t>R2PC - RESELLER 2T PC</t>
+  </si>
+  <si>
+    <t>R2PS - RESELLR 2T PTR</t>
+  </si>
+  <si>
+    <t>RCCR - RESELLER CCR</t>
+  </si>
+  <si>
+    <t>REPC - RESELLER PC</t>
+  </si>
+  <si>
+    <t>S2MR - SOL PRO 2T MIDR</t>
+  </si>
+  <si>
+    <t>SB - SHIP/INST/BILLT</t>
+  </si>
+  <si>
+    <t>SH - SHIP-TO</t>
+  </si>
+  <si>
+    <t>ST - SOLD-TO</t>
+  </si>
+  <si>
+    <t>T2 - TIER 2</t>
+  </si>
+  <si>
+    <t>U03 - CUST GRP 3 U03</t>
+  </si>
+  <si>
+    <t>U04 - CUST GRP 3 U04</t>
+  </si>
+  <si>
+    <t>WWSD - WWSD SWR DISTRI</t>
+  </si>
+  <si>
+    <t>U01 - CUST GRP 3 U01</t>
+  </si>
+  <si>
+    <t>U02 - CUST GRP 3 U02</t>
+  </si>
+  <si>
+    <t>@</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -738,9 +841,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AW502"/>
+  <dimension ref="A1:AY502"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -748,7 +851,7 @@
     <col min="31" max="39" width="20.4140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>35</v>
@@ -829,11 +932,13 @@
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
-      <c r="AW1" s="2" t="s">
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -979,49 +1084,55 @@
         <v>74</v>
       </c>
       <c r="AW2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -2491,13 +2602,25 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1CE1BAFD-C9CE-438E-A003-578944723612}">
+          <x14:formula1>
+            <xm:f>Config!$F$3:$F$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>AX3:AX1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2508,12 +2631,12 @@
     <col min="3" max="16384" width="16.58203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2527,7 +2650,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>39</v>
@@ -2539,7 +2662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2552,8 +2675,11 @@
       <c r="D4" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2566,8 +2692,11 @@
       <c r="D5" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2580,8 +2709,11 @@
       <c r="D6" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2594,8 +2726,11 @@
       <c r="D7" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -2608,8 +2743,11 @@
       <c r="D8" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2622,8 +2760,11 @@
       <c r="D9" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2636,8 +2777,11 @@
       <c r="D10" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2650,8 +2794,11 @@
       <c r="D11" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2664,8 +2811,11 @@
       <c r="D12" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2678,8 +2828,11 @@
       <c r="D13" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2692,8 +2845,11 @@
       <c r="D14" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -2706,8 +2862,11 @@
       <c r="D15" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F15" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -2720,8 +2879,11 @@
       <c r="D16" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F16" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
@@ -2734,8 +2896,11 @@
       <c r="D17" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -2748,8 +2913,11 @@
       <c r="D18" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F18" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -2762,8 +2930,11 @@
       <c r="D19" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F19" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>33</v>
@@ -2774,8 +2945,11 @@
       <c r="D20" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>47</v>
@@ -2786,8 +2960,11 @@
       <c r="D21" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F21" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>48</v>
@@ -2798,8 +2975,11 @@
       <c r="D22" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F22" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>34</v>
@@ -2810,8 +2990,11 @@
       <c r="D23" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F23" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>77</v>
@@ -2822,8 +3005,11 @@
       <c r="D24" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>19</v>
@@ -2834,8 +3020,11 @@
       <c r="D25" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F25" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>43</v>
@@ -2846,8 +3035,11 @@
       <c r="D26" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F26" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>20</v>
@@ -2858,8 +3050,11 @@
       <c r="D27" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F27" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>21</v>
@@ -2870,8 +3065,11 @@
       <c r="D28" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F28" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>22</v>
@@ -2882,8 +3080,11 @@
       <c r="D29" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F29" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>44</v>
@@ -2894,8 +3095,11 @@
       <c r="D30" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F30" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>23</v>
@@ -2906,8 +3110,11 @@
       <c r="D31" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F31" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>9</v>
@@ -3138,12 +3345,34 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="C51" s="7">
         <v>49</v>
       </c>
       <c r="D51" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="7">
+        <v>50</v>
+      </c>
+      <c r="D52" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="7">
+        <v>51</v>
+      </c>
+      <c r="D53" s="7">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CREATCMR-6255 addr2 null remove
CREATCMR-6255 addr2 null remove
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateUS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateUS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D162F5DE-5331-4E13-BC41-6CFB9617522E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB49924-B742-4157-9990-BADAADA71BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
     <t>Cmr No.</t>
   </si>
   <si>
-    <t>Division</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>Address 1</t>
-  </si>
-  <si>
-    <t>Address 2</t>
   </si>
   <si>
     <t>State/Province</t>
@@ -419,6 +413,14 @@
   </si>
   <si>
     <t>@</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Division/Address Con't</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -847,59 +849,61 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="20.4140625" style="10"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
     <col min="31" max="39" width="20.4140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -935,7 +939,7 @@
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
       <c r="AY1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -943,154 +947,154 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AG2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AF2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="AY2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.3">
@@ -2633,27 +2637,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -2664,10 +2668,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
@@ -2676,15 +2680,15 @@
         <v>70</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -2693,15 +2697,15 @@
         <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -2710,15 +2714,15 @@
         <v>70</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4">
         <v>5</v>
@@ -2727,15 +2731,15 @@
         <v>70</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4">
         <v>6</v>
@@ -2744,15 +2748,15 @@
         <v>70</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="4">
         <v>7</v>
@@ -2761,15 +2765,15 @@
         <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4">
         <v>8</v>
@@ -2778,15 +2782,15 @@
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>9</v>
@@ -2795,15 +2799,15 @@
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4">
         <v>10</v>
@@ -2812,15 +2816,15 @@
         <v>70</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4">
         <v>11</v>
@@ -2829,15 +2833,15 @@
         <v>100</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4">
         <v>12</v>
@@ -2846,15 +2850,15 @@
         <v>70</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C15" s="4">
         <v>13</v>
@@ -2863,15 +2867,15 @@
         <v>70</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4">
         <v>14</v>
@@ -2880,15 +2884,15 @@
         <v>70</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="4">
         <v>15</v>
@@ -2897,15 +2901,15 @@
         <v>50</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4">
         <v>16</v>
@@ -2914,15 +2918,15 @@
         <v>3</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4">
         <v>17</v>
@@ -2931,13 +2935,13 @@
         <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="4">
         <v>18</v>
@@ -2946,13 +2950,13 @@
         <v>15</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4">
         <v>19</v>
@@ -2961,13 +2965,13 @@
         <v>28</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="4">
         <v>20</v>
@@ -2976,13 +2980,13 @@
         <v>24</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4">
         <v>21</v>
@@ -2991,13 +2995,13 @@
         <v>4</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" s="4">
         <v>22</v>
@@ -3006,13 +3010,13 @@
         <v>3</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4">
         <v>23</v>
@@ -3021,13 +3025,13 @@
         <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4">
         <v>24</v>
@@ -3036,13 +3040,13 @@
         <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4">
         <v>25</v>
@@ -3051,13 +3055,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
         <v>26</v>
@@ -3066,13 +3070,13 @@
         <v>3</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4">
         <v>27</v>
@@ -3081,13 +3085,13 @@
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4">
         <v>28</v>
@@ -3096,13 +3100,13 @@
         <v>3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="4">
         <v>29</v>
@@ -3111,13 +3115,13 @@
         <v>3</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="4">
         <v>30</v>
@@ -3129,7 +3133,7 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4">
         <v>31</v>
@@ -3141,7 +3145,7 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34" s="4">
         <v>32</v>
@@ -3153,7 +3157,7 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C35" s="4">
         <v>33</v>
@@ -3165,7 +3169,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4">
         <v>34</v>
@@ -3177,7 +3181,7 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37" s="4">
         <v>35</v>
@@ -3189,7 +3193,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4">
         <v>36</v>
@@ -3201,7 +3205,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" s="4">
         <v>37</v>
@@ -3213,7 +3217,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="4">
         <v>38</v>
@@ -3225,7 +3229,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" s="4">
         <v>39</v>
@@ -3237,7 +3241,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42" s="4">
         <v>40</v>
@@ -3249,7 +3253,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="7">
         <v>41</v>
@@ -3261,7 +3265,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C44" s="7">
         <v>42</v>
@@ -3273,7 +3277,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C45" s="7">
         <v>43</v>
@@ -3285,7 +3289,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C46" s="7">
         <v>44</v>
@@ -3297,7 +3301,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="7">
         <v>45</v>
@@ -3309,7 +3313,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C48" s="7">
         <v>46</v>
@@ -3321,7 +3325,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49" s="7">
         <v>47</v>
@@ -3333,7 +3337,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C50" s="7">
         <v>48</v>
@@ -3345,7 +3349,7 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="7">
         <v>49</v>
@@ -3356,7 +3360,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C52" s="7">
         <v>50</v>
@@ -3367,7 +3371,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C53" s="7">
         <v>51</v>

</xml_diff>